<commit_message>
peta, kmeansm pca done
</commit_message>
<xml_diff>
--- a/Data CSV/analisis.xlsx
+++ b/Data CSV/analisis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\clone pca\ta_elaine\Data CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3D62993-D509-48E0-898C-84FF2501A0BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B380AE-73E1-4F12-95F1-7C9CAD61D25F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{B73A4F9A-491E-4439-9728-3A59325EE64F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{B73A4F9A-491E-4439-9728-3A59325EE64F}"/>
   </bookViews>
   <sheets>
     <sheet name="analisis_gr" sheetId="1" r:id="rId1"/>
@@ -3721,7 +3721,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B8DF412-7B5D-44AA-A240-9A8CDA41E4CA}">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+    <sheetView topLeftCell="A42" workbookViewId="0">
       <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
@@ -4333,10 +4333,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F69A1A67-3BDB-4145-8BFF-43AA850D1DFF}">
-  <dimension ref="A1:BC595"/>
+  <dimension ref="A1:BF595"/>
   <sheetViews>
-    <sheetView topLeftCell="AS1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="BE11" sqref="BE11"/>
+    <sheetView tabSelected="1" topLeftCell="AV1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="BF2" sqref="BF2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -4345,7 +4345,7 @@
     <col min="6" max="6" width="14.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55">
+    <row r="1" spans="1:58">
       <c r="A1" t="s">
         <v>84</v>
       </c>
@@ -4464,7 +4464,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="2" spans="1:55">
+    <row r="2" spans="1:58">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4625,8 +4625,11 @@
         <f>"('"&amp;BA2&amp;"','"&amp;BB2&amp;"'),"</f>
         <v>('13','i2023110600334'),</v>
       </c>
-    </row>
-    <row r="3" spans="1:55">
+      <c r="BF2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:58">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4788,7 +4791,7 @@
         <v>('13','i2023110600335'),</v>
       </c>
     </row>
-    <row r="4" spans="1:55">
+    <row r="4" spans="1:58">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4950,7 +4953,7 @@
         <v>('13','i2023110600336'),</v>
       </c>
     </row>
-    <row r="5" spans="1:55">
+    <row r="5" spans="1:58">
       <c r="A5">
         <v>3</v>
       </c>
@@ -5112,7 +5115,7 @@
         <v>('13','i2023110600337'),</v>
       </c>
     </row>
-    <row r="6" spans="1:55">
+    <row r="6" spans="1:58">
       <c r="A6">
         <v>3</v>
       </c>
@@ -5274,7 +5277,7 @@
         <v>('13','i2023110600338'),</v>
       </c>
     </row>
-    <row r="7" spans="1:55">
+    <row r="7" spans="1:58">
       <c r="A7">
         <v>3</v>
       </c>
@@ -5436,7 +5439,7 @@
         <v>('13','i2023110600339'),</v>
       </c>
     </row>
-    <row r="8" spans="1:55">
+    <row r="8" spans="1:58">
       <c r="A8">
         <v>3</v>
       </c>
@@ -5598,7 +5601,7 @@
         <v>('13','i2023110600340'),</v>
       </c>
     </row>
-    <row r="9" spans="1:55">
+    <row r="9" spans="1:58">
       <c r="A9">
         <v>3</v>
       </c>
@@ -5760,7 +5763,7 @@
         <v>('13','i2023110600341'),</v>
       </c>
     </row>
-    <row r="10" spans="1:55">
+    <row r="10" spans="1:58">
       <c r="A10">
         <v>3</v>
       </c>
@@ -5922,7 +5925,7 @@
         <v>('13','i2023110600342'),</v>
       </c>
     </row>
-    <row r="11" spans="1:55">
+    <row r="11" spans="1:58">
       <c r="A11">
         <v>3</v>
       </c>
@@ -6084,7 +6087,7 @@
         <v>('13','i2023110600343'),</v>
       </c>
     </row>
-    <row r="12" spans="1:55">
+    <row r="12" spans="1:58">
       <c r="A12">
         <v>3</v>
       </c>
@@ -6246,7 +6249,7 @@
         <v>('13','i2023110600344'),</v>
       </c>
     </row>
-    <row r="13" spans="1:55">
+    <row r="13" spans="1:58">
       <c r="A13">
         <v>3</v>
       </c>
@@ -6408,7 +6411,7 @@
         <v>('13','i2023110600345'),</v>
       </c>
     </row>
-    <row r="14" spans="1:55">
+    <row r="14" spans="1:58">
       <c r="A14">
         <v>3</v>
       </c>
@@ -6570,7 +6573,7 @@
         <v>('13','i2023110600346'),</v>
       </c>
     </row>
-    <row r="15" spans="1:55">
+    <row r="15" spans="1:58">
       <c r="A15">
         <v>3</v>
       </c>
@@ -6732,7 +6735,7 @@
         <v>('13','i2023110600347'),</v>
       </c>
     </row>
-    <row r="16" spans="1:55">
+    <row r="16" spans="1:58">
       <c r="A16">
         <v>3</v>
       </c>
@@ -24238,7 +24241,7 @@
         <v>612</v>
       </c>
       <c r="BC195" t="str">
-        <f t="shared" ref="BC195:BC245" si="42">"('"&amp;BA195&amp;"','"&amp;BB195&amp;"'),"</f>
+        <f t="shared" ref="BC195:BC243" si="42">"('"&amp;BA195&amp;"','"&amp;BB195&amp;"'),"</f>
         <v>('13','i2023110600527'),</v>
       </c>
     </row>

</xml_diff>